<commit_message>
Korjaa excelin tuonti ja viento toisen asteen koulutukselle
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_syntymaajalla.xlsx
+++ b/src/test/resources/erillishaku_syntymaajalla.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Ilmoittautumistila</t>
   </si>
   <si>
-    <t xml:space="preserve">Lukuvuosimaksuvelvollisuus</t>
+    <t xml:space="preserve">Maksuvelvollisuus</t>
   </si>
   <si>
     <t xml:space="preserve">Julkaistavissa</t>
@@ -299,15 +299,15 @@
   </sheetPr>
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="15" min="1" style="1" width="13.2962962962963"/>
-    <col collapsed="false" hidden="false" max="260" min="16" style="1" width="9.92222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="261" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="15" min="1" style="1" width="14.4111111111111"/>
+    <col collapsed="false" hidden="false" max="260" min="16" style="1" width="10.7"/>
+    <col collapsed="false" hidden="false" max="1025" min="261" style="0" width="11.3074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>